<commit_message>
im commiting through the git bash
</commit_message>
<xml_diff>
--- a/GUISeleniumFramework/testdata/testScriptdata.xlsx
+++ b/GUISeleniumFramework/testdata/testScriptdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="160">
   <si>
     <t>TC_ID</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Bharath2669</t>
+  </si>
+  <si>
+    <t>Bharath652</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1070,7 @@
         <v>148</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>